<commit_message>
DAX and EP Global Objects
</commit_message>
<xml_diff>
--- a/DesktopClient/TC_CreateGeneralJournal/Main.rvl.xlsx
+++ b/DesktopClient/TC_CreateGeneralJournal/Main.rvl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="149">
   <si>
     <t>Offset account</t>
   </si>
@@ -439,6 +439,30 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>DAX</t>
+  </si>
+  <si>
+    <t>Launch</t>
+  </si>
+  <si>
+    <t>ChangeCompany</t>
+  </si>
+  <si>
+    <t>OpenModule</t>
+  </si>
+  <si>
+    <t>Navigate</t>
+  </si>
+  <si>
+    <t>OpenDropdown</t>
+  </si>
+  <si>
+    <t>ClickCell</t>
+  </si>
+  <si>
+    <t>yOffset</t>
   </si>
 </sst>
 </file>
@@ -462,7 +486,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="68">
     <border outline="false">
       <left/>
       <right/>
@@ -489,11 +513,59 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
@@ -515,6 +587,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="true"/>
@@ -813,7 +933,7 @@
     <outlinePr/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection activeCell="$A$1" sqref="$A$1:$A$1"/>
@@ -1003,112 +1123,119 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1"/>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="1"/>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" t="s">
-        <v>35</v>
-      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" t="s">
+        <v>143</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
@@ -1116,66 +1243,67 @@
         <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="G20" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="B21" t="s">
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
         <v>47</v>
       </c>
       <c r="G21" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1"/>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1"/>
@@ -1183,46 +1311,56 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="G24" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="F25" t="s">
         <v>47</v>
       </c>
       <c r="G25" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1"/>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1"/>
@@ -1230,208 +1368,199 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="G27" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1"/>
       <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
         <v>49</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>101</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>13</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>26</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1"/>
-      <c r="B29" t="s">
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" t="s">
         <v>24</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>47</v>
       </c>
-      <c r="G29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1"/>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" t="s">
-        <v>110</v>
-      </c>
-      <c r="E30" t="s">
-        <v>100</v>
-      </c>
-      <c r="F30" t="s">
-        <v>99</v>
-      </c>
       <c r="G30" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="E31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="1"/>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" t="s">
         <v>13</v>
       </c>
-      <c r="F31" t="s">
-        <v>93</v>
-      </c>
-      <c r="G31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1"/>
-      <c r="B32" t="s">
+      <c r="F34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1"/>
+      <c r="B35" t="s">
         <v>1</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E35" t="s">
         <v>24</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F35" t="s">
         <v>47</v>
       </c>
-      <c r="G32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" t="s">
-        <v>47</v>
-      </c>
-      <c r="G34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" t="s">
-        <v>90</v>
-      </c>
-      <c r="F35" t="s">
-        <v>90</v>
-      </c>
       <c r="G35" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="A36" s="1"/>
       <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="F36" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G36" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1"/>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1"/>
@@ -1439,19 +1568,19 @@
         <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F38" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G38" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39">
@@ -1460,86 +1589,87 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="F39" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="G39" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1"/>
-      <c r="B40" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="41">
-      <c r="A41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="B41" t="s">
         <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D41" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="E41" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="F41" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="G41" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1"/>
+      <c r="A42" s="13"/>
       <c r="B42" t="s">
         <v>32</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F42" t="s">
         <v>47</v>
       </c>
       <c r="G42" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1"/>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>68</v>
-      </c>
-      <c r="F43" t="s">
-        <v>96</v>
-      </c>
-      <c r="G43" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="44">
-      <c r="A44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
@@ -1549,66 +1679,84 @@
         <v>32</v>
       </c>
       <c r="C45" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="D45" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="E45" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="F45" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="G45" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="13"/>
+      <c r="A46" s="17"/>
       <c r="B46" t="s">
         <v>32</v>
       </c>
       <c r="C46" t="s">
-        <v>131</v>
+        <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E46" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F46" t="s">
         <v>47</v>
       </c>
       <c r="G46" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1"/>
+      <c r="A47" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="A48" s="19"/>
       <c r="B48" t="s">
         <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="F48" t="s">
         <v>47</v>
       </c>
       <c r="G48" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49">
@@ -1619,31 +1767,33 @@
         <v>32</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>101</v>
       </c>
       <c r="E49" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="F49" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="G49" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="17"/>
+      <c r="A50" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="B50" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
       <c r="E50" t="s">
         <v>24</v>
@@ -1656,188 +1806,138 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B51" t="s">
         <v>32</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="D51" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E51" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="F51" t="s">
         <v>47</v>
       </c>
       <c r="G51" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="19"/>
+      <c r="A52" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="B52" t="s">
         <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D52" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="E52" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="F52" t="s">
+        <v>90</v>
+      </c>
+      <c r="G52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G52" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" t="s">
-        <v>101</v>
-      </c>
-      <c r="E53" t="s">
-        <v>13</v>
-      </c>
-      <c r="F53" t="s">
-        <v>26</v>
-      </c>
-      <c r="G53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" t="s">
-        <v>90</v>
-      </c>
-      <c r="E54" t="s">
-        <v>24</v>
-      </c>
-      <c r="F54" t="s">
-        <v>47</v>
-      </c>
-      <c r="G54" t="s">
-        <v>89</v>
-      </c>
+      <c r="G54" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H54" s="1"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B55" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" t="s">
-        <v>85</v>
-      </c>
-      <c r="E55" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55" t="s">
-        <v>47</v>
-      </c>
-      <c r="G55" t="s">
-        <v>95</v>
-      </c>
+      <c r="B55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H55" s="1"/>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B56" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" t="s">
-        <v>23</v>
-      </c>
-      <c r="E56" t="s">
-        <v>90</v>
-      </c>
-      <c r="F56" t="s">
-        <v>90</v>
-      </c>
-      <c r="G56" t="s">
-        <v>90</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
     </row>
     <row r="57">
       <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
     </row>
     <row r="58">
       <c r="A58" s="1"/>
-      <c r="B58" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
     <row r="60">
@@ -1929,46 +2029,6 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
     </row>
   </sheetData>
   <sheetProtection/>
@@ -2330,10 +2390,10 @@
         <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>100</v>
@@ -2347,58 +2407,49 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" t="s">
         <v>99</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="1"/>
     </row>
     <row r="22">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="42"/>
+      <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="1"/>
     </row>
     <row r="23">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
+      <c r="A23" s="43"/>
+      <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="1"/>
@@ -2428,10 +2479,10 @@
         <v>32</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>100</v>
@@ -2445,58 +2496,49 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="51"/>
+      <c r="B26" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" t="s">
         <v>99</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" t="s">
         <v>42</v>
       </c>
-      <c r="H26" s="1"/>
     </row>
     <row r="27">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
+      <c r="A27" s="52"/>
+      <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" t="s">
         <v>73</v>
       </c>
-      <c r="H27" s="1"/>
     </row>
     <row r="28">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
+      <c r="A28" s="53"/>
+      <c r="B28" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" t="s">
         <v>47</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="1"/>
     </row>
     <row r="29">
       <c r="A29" s="1"/>
@@ -2526,10 +2568,10 @@
         <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>100</v>
@@ -2543,94 +2585,79 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1" t="s">
+      <c r="A31" s="61"/>
+      <c r="B31" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" t="s">
         <v>99</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" t="s">
         <v>84</v>
       </c>
-      <c r="H31" s="1"/>
     </row>
     <row r="32">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
+      <c r="A32" s="62"/>
+      <c r="B32" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" t="s">
         <v>26</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="1"/>
     </row>
     <row r="33">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1" t="s">
+      <c r="A33" s="63"/>
+      <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" t="s">
         <v>0</v>
       </c>
-      <c r="H33" s="1"/>
     </row>
     <row r="34">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1" t="s">
+      <c r="A34" s="64"/>
+      <c r="B34" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" t="s">
         <v>47</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="1"/>
     </row>
     <row r="35">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
+      <c r="A35" s="65"/>
+      <c r="B35" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>65</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" t="s">
         <v>26</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" t="s">
         <v>31</v>
       </c>
-      <c r="H35" s="1"/>
     </row>
     <row r="36">
       <c r="A36" s="1"/>

</xml_diff>